<commit_message>
Performed cluster analysis on new grid of Area 2
</commit_message>
<xml_diff>
--- a/_CLUSTER/groups_time_area/interpolation/Area2/control_points_count.xlsx
+++ b/_CLUSTER/groups_time_area/interpolation/Area2/control_points_count.xlsx
@@ -379,18 +379,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>41172</v>
+        <v>26582</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>39825</v>
+        <v>20457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>